<commit_message>
rand forest and tsne updates
</commit_message>
<xml_diff>
--- a/models/Random Forests/All_Meta/metrics.xlsx
+++ b/models/Random Forests/All_Meta/metrics.xlsx
@@ -500,40 +500,40 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.731668159196355</v>
+        <v>0.7441320593187497</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9995586357148223</v>
+        <v>0.9995917744288552</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8422726598399318</v>
+        <v>0.857921434222939</v>
       </c>
       <c r="E2" t="n">
-        <v>0.795073572630407</v>
+        <v>0.8166022341605902</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7865857969151671</v>
+        <v>0.7569633676092544</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9266095421411318</v>
+        <v>0.9277736891103059</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9059051802211712</v>
+        <v>0.9008891064586511</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8224127543573576</v>
+        <v>0.8280243026161923</v>
       </c>
       <c r="J2" t="n">
-        <v>0.9079750041354273</v>
+        <v>0.9143653571891611</v>
       </c>
       <c r="K2" t="n">
-        <v>0.894833995171589</v>
+        <v>0.889498276776246</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9202483395104766</v>
+        <v>0.9017421379031961</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9224101970168628</v>
+        <v>0.9175424284798955</v>
       </c>
     </row>
     <row r="3">
@@ -541,40 +541,40 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.7366849200493082</v>
+        <v>0.7371857750608142</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9996314495472927</v>
+        <v>0.999636073553902</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8474145833967317</v>
+        <v>0.8485058275767626</v>
       </c>
       <c r="E3" t="n">
-        <v>0.792229432002677</v>
+        <v>0.807192422457763</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8149509961439588</v>
+        <v>0.7990014460154241</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9228861589170693</v>
+        <v>0.9274308700684379</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9050199396316305</v>
+        <v>0.9002636175239414</v>
       </c>
       <c r="I3" t="n">
-        <v>0.816671487089115</v>
+        <v>0.8174478793824608</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9111395375176407</v>
+        <v>0.9143765340200378</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9009650476072291</v>
+        <v>0.8967602829358544</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9344106638288503</v>
+        <v>0.9027237532567611</v>
       </c>
       <c r="M3" t="n">
-        <v>0.9301762681591084</v>
+        <v>0.9214871096761912</v>
       </c>
     </row>
     <row r="4">
@@ -582,40 +582,40 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.7242576945561713</v>
+        <v>0.7398099268915896</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9995537833622077</v>
+        <v>0.9995858945192163</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8529454558595295</v>
+        <v>0.8514400619275129</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8252790759609941</v>
+        <v>0.8359218921183218</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7399831298200514</v>
+        <v>0.797036471722365</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9260065760150679</v>
+        <v>0.9218801669973544</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8969650321279785</v>
+        <v>0.9087481143028904</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8196276391812906</v>
+        <v>0.8182579025300972</v>
       </c>
       <c r="J4" t="n">
-        <v>0.9168585355967162</v>
+        <v>0.9122665346310378</v>
       </c>
       <c r="K4" t="n">
-        <v>0.8910011619773923</v>
+        <v>0.8890103590848583</v>
       </c>
       <c r="L4" t="n">
-        <v>0.9177014146269862</v>
+        <v>0.8836648196396462</v>
       </c>
       <c r="M4" t="n">
-        <v>0.9267953409961294</v>
+        <v>0.9283160395528551</v>
       </c>
     </row>
     <row r="5">
@@ -623,40 +623,40 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.7363778384520898</v>
+        <v>0.730267954694243</v>
       </c>
       <c r="C5" t="n">
-        <v>0.9995425658646927</v>
+        <v>0.9996031917291252</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8448407686923709</v>
+        <v>0.8383204064088128</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8083935924143827</v>
+        <v>0.8225630497759552</v>
       </c>
       <c r="F5" t="n">
-        <v>0.833288881748072</v>
+        <v>0.8004305912596401</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9224022583822177</v>
+        <v>0.9237238864446745</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9061106359615307</v>
+        <v>0.9083146157217512</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8243940921158707</v>
+        <v>0.823188185769152</v>
       </c>
       <c r="J5" t="n">
-        <v>0.9080323785339278</v>
+        <v>0.9084157438329973</v>
       </c>
       <c r="K5" t="n">
-        <v>0.888644773358002</v>
+        <v>0.8903186412761445</v>
       </c>
       <c r="L5" t="n">
-        <v>0.8967904847528529</v>
+        <v>0.8816213166489302</v>
       </c>
       <c r="M5" t="n">
-        <v>0.9245968599698864</v>
+        <v>0.9146501946149194</v>
       </c>
     </row>
     <row r="6">
@@ -664,40 +664,40 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.7510060890832219</v>
+        <v>0.7320967597143977</v>
       </c>
       <c r="C6" t="n">
-        <v>0.9996023925181062</v>
+        <v>0.9995634309809356</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8474835291074526</v>
+        <v>0.8536349129667387</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8096770661947915</v>
+        <v>0.8165106129227874</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7901341580976864</v>
+        <v>0.781844473007712</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9199982567000231</v>
+        <v>0.9253016178542675</v>
       </c>
       <c r="H6" t="n">
-        <v>0.89908778520015</v>
+        <v>0.902256929136013</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8146742947850075</v>
+        <v>0.8344343434440493</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9068452128143112</v>
+        <v>0.9124027056872186</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8866804110918075</v>
+        <v>0.8976092033121996</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9330081923599134</v>
+        <v>0.8635933085024403</v>
       </c>
       <c r="M6" t="n">
-        <v>0.9243279189522927</v>
+        <v>0.9162983367179868</v>
       </c>
     </row>
     <row r="7">
@@ -705,40 +705,40 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.738108114617522</v>
+        <v>0.7349064742215674</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9996455213698752</v>
+        <v>0.9996595075627055</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8491120743434465</v>
+        <v>0.8560133022427803</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8132231186782316</v>
+        <v>0.7940797151355956</v>
       </c>
       <c r="F7" t="n">
-        <v>0.7428767673521851</v>
+        <v>0.7870629820051414</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9204826065389924</v>
+        <v>0.9181520660800552</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9045195484838626</v>
+        <v>0.8903934890076837</v>
       </c>
       <c r="I7" t="n">
-        <v>0.8197842628741312</v>
+        <v>0.8164504843323459</v>
       </c>
       <c r="J7" t="n">
-        <v>0.9099259199649494</v>
+        <v>0.9114347921332993</v>
       </c>
       <c r="K7" t="n">
-        <v>0.8839510333701858</v>
+        <v>0.8886183327316622</v>
       </c>
       <c r="L7" t="n">
-        <v>0.9349748633077686</v>
+        <v>0.9172702377894389</v>
       </c>
       <c r="M7" t="n">
-        <v>0.923815908915235</v>
+        <v>0.9177874139436655</v>
       </c>
     </row>
     <row r="8">
@@ -746,40 +746,40 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.7308098633952167</v>
+        <v>0.7342452361298741</v>
       </c>
       <c r="C8" t="n">
-        <v>0.9996075017599768</v>
+        <v>0.9995815559451139</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8520596223486808</v>
+        <v>0.8422279639998783</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8039025988597037</v>
+        <v>0.7712062401827455</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7740311696658098</v>
+        <v>0.7904330012853471</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9223141947751322</v>
+        <v>0.9188601693696803</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9012370346785834</v>
+        <v>0.902832900196725</v>
       </c>
       <c r="I8" t="n">
-        <v>0.8154655807423963</v>
+        <v>0.812349441871951</v>
       </c>
       <c r="J8" t="n">
-        <v>0.9079625233409485</v>
+        <v>0.9139270391382812</v>
       </c>
       <c r="K8" t="n">
-        <v>0.8965769612598994</v>
+        <v>0.8924825421357822</v>
       </c>
       <c r="L8" t="n">
-        <v>0.8638146306557558</v>
+        <v>0.9840980606216285</v>
       </c>
       <c r="M8" t="n">
-        <v>0.918579863664152</v>
+        <v>0.9186996414332703</v>
       </c>
     </row>
     <row r="9">
@@ -787,40 +787,40 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.7319976834771489</v>
+        <v>0.7358446878715359</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9995527558051834</v>
+        <v>0.9996131533236104</v>
       </c>
       <c r="D9" t="n">
-        <v>0.8476489988131828</v>
+        <v>0.8533752967043</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8262938976373367</v>
+        <v>0.7925066250695895</v>
       </c>
       <c r="F9" t="n">
-        <v>0.7585258676092546</v>
+        <v>0.7904105077120822</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9211882386559698</v>
+        <v>0.922302288216011</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8980314038881956</v>
+        <v>0.9000720615376863</v>
       </c>
       <c r="I9" t="n">
-        <v>0.823055103674315</v>
+        <v>0.8150206925842044</v>
       </c>
       <c r="J9" t="n">
-        <v>0.9094473653229135</v>
+        <v>0.9155828866326593</v>
       </c>
       <c r="K9" t="n">
-        <v>0.8924247252995193</v>
+        <v>0.8943629994810586</v>
       </c>
       <c r="L9" t="n">
-        <v>0.9188722432204321</v>
+        <v>0.8998672067080108</v>
       </c>
       <c r="M9" t="n">
-        <v>0.9206553728474336</v>
+        <v>0.9322795657848255</v>
       </c>
     </row>
     <row r="10">
@@ -828,40 +828,40 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.7241142803342975</v>
+        <v>0.7365376741497507</v>
       </c>
       <c r="C10" t="n">
-        <v>0.999657623708161</v>
+        <v>0.9995925450966234</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8520130245579868</v>
+        <v>0.8497639679255045</v>
       </c>
       <c r="E10" t="n">
-        <v>0.8162714659630983</v>
+        <v>0.8119039281441031</v>
       </c>
       <c r="F10" t="n">
-        <v>0.7718942802056554</v>
+        <v>0.7905004820051413</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9230312841471129</v>
+        <v>0.9241075921612607</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9016323089359346</v>
+        <v>0.9072890744892167</v>
       </c>
       <c r="I10" t="n">
-        <v>0.8062036434706656</v>
+        <v>0.8147184953363613</v>
       </c>
       <c r="J10" t="n">
-        <v>0.9153854292871715</v>
+        <v>0.9079098059553137</v>
       </c>
       <c r="K10" t="n">
-        <v>0.8909197248482661</v>
+        <v>0.8899812588840506</v>
       </c>
       <c r="L10" t="n">
-        <v>0.9172966129683314</v>
+        <v>0.9361674800924736</v>
       </c>
       <c r="M10" t="n">
-        <v>0.915284857087554</v>
+        <v>0.9160664469569739</v>
       </c>
     </row>
     <row r="11">
@@ -869,40 +869,40 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.7390884767220107</v>
+        <v>0.749696202697939</v>
       </c>
       <c r="C11" t="n">
-        <v>0.9996481188056864</v>
+        <v>0.9995657429842402</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8396008946775813</v>
+        <v>0.8437148139131494</v>
       </c>
       <c r="E11" t="n">
-        <v>0.7738617031766947</v>
+        <v>0.8132301067387421</v>
       </c>
       <c r="F11" t="n">
-        <v>0.7744424807197944</v>
+        <v>0.80188544344473</v>
       </c>
       <c r="G11" t="n">
-        <v>0.921420753536922</v>
+        <v>0.91993400621118</v>
       </c>
       <c r="H11" t="n">
-        <v>0.8984953081814386</v>
+        <v>0.9034705514162763</v>
       </c>
       <c r="I11" t="n">
-        <v>0.8191222154853749</v>
+        <v>0.8160709361196337</v>
       </c>
       <c r="J11" t="n">
-        <v>0.9066390002846366</v>
+        <v>0.9072628537280691</v>
       </c>
       <c r="K11" t="n">
-        <v>0.8964972868391959</v>
+        <v>0.8896445815753256</v>
       </c>
       <c r="L11" t="n">
-        <v>0.8973478037503211</v>
+        <v>0.900788044475432</v>
       </c>
       <c r="M11" t="n">
-        <v>0.9231774135539885</v>
+        <v>0.917396139897879</v>
       </c>
     </row>
     <row r="12">
@@ -910,40 +910,40 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.7349294642876693</v>
+        <v>0.711999062881115</v>
       </c>
       <c r="C12" t="n">
-        <v>0.9996235430668557</v>
+        <v>0.9995603768531134</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8521637541462523</v>
+        <v>0.8530790678920299</v>
       </c>
       <c r="E12" t="n">
-        <v>0.8181411603752122</v>
+        <v>0.7960006553247857</v>
       </c>
       <c r="F12" t="n">
-        <v>0.7971079691516709</v>
+        <v>0.7591171272493573</v>
       </c>
       <c r="G12" t="n">
-        <v>0.9179222470238095</v>
+        <v>0.9226976758396594</v>
       </c>
       <c r="H12" t="n">
-        <v>0.9057718294552296</v>
+        <v>0.9060389653544285</v>
       </c>
       <c r="I12" t="n">
-        <v>0.8161982529251637</v>
+        <v>0.822826894305912</v>
       </c>
       <c r="J12" t="n">
-        <v>0.911099673487514</v>
+        <v>0.9076808672028565</v>
       </c>
       <c r="K12" t="n">
-        <v>0.8883909433451411</v>
+        <v>0.8883380620924618</v>
       </c>
       <c r="L12" t="n">
-        <v>0.9164010036328942</v>
+        <v>0.9163952698983524</v>
       </c>
       <c r="M12" t="n">
-        <v>0.9239420748320397</v>
+        <v>0.9175938530687704</v>
       </c>
     </row>
     <row r="13">
@@ -951,40 +951,40 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.7257498593226908</v>
+        <v>0.7319434926070516</v>
       </c>
       <c r="C13" t="n">
-        <v>0.9996527998987971</v>
+        <v>0.9996537132828186</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8465415880527069</v>
+        <v>0.8516430951583944</v>
       </c>
       <c r="E13" t="n">
-        <v>0.8177257590004279</v>
+        <v>0.8135189465731717</v>
       </c>
       <c r="F13" t="n">
-        <v>0.8418396529562981</v>
+        <v>0.7748481683804627</v>
       </c>
       <c r="G13" t="n">
-        <v>0.9212010438233265</v>
+        <v>0.919758552953186</v>
       </c>
       <c r="H13" t="n">
-        <v>0.9004412737560916</v>
+        <v>0.902291244153959</v>
       </c>
       <c r="I13" t="n">
-        <v>0.8243431653936587</v>
+        <v>0.8046566241732815</v>
       </c>
       <c r="J13" t="n">
-        <v>0.9096494796812666</v>
+        <v>0.9172728234612112</v>
       </c>
       <c r="K13" t="n">
-        <v>0.8911742599444958</v>
+        <v>0.8915909642156088</v>
       </c>
       <c r="L13" t="n">
-        <v>0.9000827951267842</v>
+        <v>0.8830272283585923</v>
       </c>
       <c r="M13" t="n">
-        <v>0.9201475151063722</v>
+        <v>0.9264139685792567</v>
       </c>
     </row>
     <row r="14">
@@ -992,40 +992,40 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.7230282734022451</v>
+        <v>0.7476632239954983</v>
       </c>
       <c r="C14" t="n">
-        <v>0.999610213368791</v>
+        <v>0.9996385568167105</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8497192720854508</v>
+        <v>0.842816617723137</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8159717558123194</v>
+        <v>0.7981576366689934</v>
       </c>
       <c r="F14" t="n">
-        <v>0.7747340938303342</v>
+        <v>0.7925401670951158</v>
       </c>
       <c r="G14" t="n">
-        <v>0.9263783751725327</v>
+        <v>0.9224292166292845</v>
       </c>
       <c r="H14" t="n">
-        <v>0.9024658598148987</v>
+        <v>0.9003070542555182</v>
       </c>
       <c r="I14" t="n">
-        <v>0.8099717404735801</v>
+        <v>0.8133871939472149</v>
       </c>
       <c r="J14" t="n">
-        <v>0.9093583232369294</v>
+        <v>0.9117086244897776</v>
       </c>
       <c r="K14" t="n">
-        <v>0.8930899714582253</v>
+        <v>0.8946735887051285</v>
       </c>
       <c r="L14" t="n">
-        <v>0.8997961083996917</v>
+        <v>0.9193630508972148</v>
       </c>
       <c r="M14" t="n">
-        <v>0.9169566353370611</v>
+        <v>0.9198859204586178</v>
       </c>
     </row>
     <row r="15">
@@ -1033,40 +1033,40 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.7281046989505583</v>
+        <v>0.722258106187831</v>
       </c>
       <c r="C15" t="n">
-        <v>0.9995925736398741</v>
+        <v>0.999596969300478</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8461516881713886</v>
+        <v>0.8443286684823954</v>
       </c>
       <c r="E15" t="n">
-        <v>0.8087919118634751</v>
+        <v>0.8020973498945191</v>
       </c>
       <c r="F15" t="n">
-        <v>0.7711873393316195</v>
+        <v>0.812538560411311</v>
       </c>
       <c r="G15" t="n">
-        <v>0.9220129363641592</v>
+        <v>0.9209465130406027</v>
       </c>
       <c r="H15" t="n">
-        <v>0.9014998269046246</v>
+        <v>0.909991273560626</v>
       </c>
       <c r="I15" t="n">
-        <v>0.8234471433471925</v>
+        <v>0.8273204568799599</v>
       </c>
       <c r="J15" t="n">
-        <v>0.9083496142503104</v>
+        <v>0.9126310855981318</v>
       </c>
       <c r="K15" t="n">
-        <v>0.8877567208546737</v>
+        <v>0.8908037386340563</v>
       </c>
       <c r="L15" t="n">
-        <v>0.933484092326887</v>
+        <v>0.8778290246229495</v>
       </c>
       <c r="M15" t="n">
-        <v>0.9089257754732181</v>
+        <v>0.9230739255614702</v>
       </c>
     </row>
     <row r="16">
@@ -1074,40 +1074,40 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.73411058002842</v>
+        <v>0.7306199216586128</v>
       </c>
       <c r="C16" t="n">
-        <v>0.9996167497731953</v>
+        <v>0.9996075017599769</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8469695269468367</v>
+        <v>0.8425089772070236</v>
       </c>
       <c r="E16" t="n">
-        <v>0.8126966847864486</v>
+        <v>0.8149491696242986</v>
       </c>
       <c r="F16" t="n">
-        <v>0.7471947300771209</v>
+        <v>0.7965223329048843</v>
       </c>
       <c r="G16" t="n">
-        <v>0.9228805426155969</v>
+        <v>0.9182062072262479</v>
       </c>
       <c r="H16" t="n">
-        <v>0.8929771058018876</v>
+        <v>0.8973029698996482</v>
       </c>
       <c r="I16" t="n">
-        <v>0.8021520864101561</v>
+        <v>0.8196406110822313</v>
       </c>
       <c r="J16" t="n">
-        <v>0.9072300683574976</v>
+        <v>0.9169133020680118</v>
       </c>
       <c r="K16" t="n">
-        <v>0.8889832133751495</v>
+        <v>0.8882880011732588</v>
       </c>
       <c r="L16" t="n">
-        <v>0.9144526806355731</v>
+        <v>0.9014588914168287</v>
       </c>
       <c r="M16" t="n">
-        <v>0.9218981869798051</v>
+        <v>0.9215698361887288</v>
       </c>
     </row>
     <row r="17">
@@ -1115,40 +1115,40 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.7346097928923473</v>
+        <v>0.7289224884447549</v>
       </c>
       <c r="C17" t="n">
-        <v>0.9996534278503119</v>
+        <v>0.9996666719186248</v>
       </c>
       <c r="D17" t="n">
-        <v>0.8368050272359332</v>
+        <v>0.8550414054654454</v>
       </c>
       <c r="E17" t="n">
-        <v>0.7916284587987835</v>
+        <v>0.8197554023531129</v>
       </c>
       <c r="F17" t="n">
-        <v>0.7716669344473007</v>
+        <v>0.799146850899743</v>
       </c>
       <c r="G17" t="n">
-        <v>0.9243765006757534</v>
+        <v>0.9170142034017714</v>
       </c>
       <c r="H17" t="n">
-        <v>0.8958656484517629</v>
+        <v>0.8944860978568751</v>
       </c>
       <c r="I17" t="n">
-        <v>0.8115221228563934</v>
+        <v>0.8222777504994181</v>
       </c>
       <c r="J17" t="n">
-        <v>0.913619676289173</v>
+        <v>0.9130971594456888</v>
       </c>
       <c r="K17" t="n">
-        <v>0.8881639065003046</v>
+        <v>0.8939878951287201</v>
       </c>
       <c r="L17" t="n">
-        <v>0.9182702010935379</v>
+        <v>0.9196508843712158</v>
       </c>
       <c r="M17" t="n">
-        <v>0.9221763908115439</v>
+        <v>0.9264797665004258</v>
       </c>
     </row>
     <row r="18">
@@ -1156,40 +1156,40 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.7519295234049821</v>
+        <v>0.7318367530144356</v>
       </c>
       <c r="C18" t="n">
-        <v>0.9995971120167314</v>
+        <v>0.9995940864321599</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8499446532363593</v>
+        <v>0.8578776893582059</v>
       </c>
       <c r="E18" t="n">
-        <v>0.7967677890785931</v>
+        <v>0.8392140450698844</v>
       </c>
       <c r="F18" t="n">
-        <v>0.7790705334190232</v>
+        <v>0.7947188303341902</v>
       </c>
       <c r="G18" t="n">
-        <v>0.9230901429865424</v>
+        <v>0.9273749317057741</v>
       </c>
       <c r="H18" t="n">
-        <v>0.9057831230054395</v>
+        <v>0.9025531676453684</v>
       </c>
       <c r="I18" t="n">
-        <v>0.8284701516559352</v>
+        <v>0.8131753195651819</v>
       </c>
       <c r="J18" t="n">
-        <v>0.9085241590925008</v>
+        <v>0.9112190792973798</v>
       </c>
       <c r="K18" t="n">
-        <v>0.8861755713995623</v>
+        <v>0.8927416602739108</v>
       </c>
       <c r="L18" t="n">
-        <v>0.9143162177534769</v>
+        <v>0.8818116766357197</v>
       </c>
       <c r="M18" t="n">
-        <v>0.9256937049276255</v>
+        <v>0.9197124822489346</v>
       </c>
     </row>
     <row r="19">
@@ -1197,40 +1197,40 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.7392258697360958</v>
+        <v>0.7467217260503722</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9996205745687857</v>
+        <v>0.9995630599186769</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8595880184717446</v>
+        <v>0.8568192538267247</v>
       </c>
       <c r="E19" t="n">
-        <v>0.8018131687670965</v>
+        <v>0.8210559580592137</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8034993573264781</v>
+        <v>0.8238174807197942</v>
       </c>
       <c r="G19" t="n">
-        <v>0.9231069918909592</v>
+        <v>0.9207966701173222</v>
       </c>
       <c r="H19" t="n">
-        <v>0.8994665534995021</v>
+        <v>0.8966496814567289</v>
       </c>
       <c r="I19" t="n">
-        <v>0.818408760933631</v>
+        <v>0.815009642446366</v>
       </c>
       <c r="J19" t="n">
-        <v>0.9112041768562107</v>
+        <v>0.9098640748340987</v>
       </c>
       <c r="K19" t="n">
-        <v>0.8879470933643194</v>
+        <v>0.8995161012838157</v>
       </c>
       <c r="L19" t="n">
-        <v>0.8626415085684929</v>
+        <v>0.9012008733624455</v>
       </c>
       <c r="M19" t="n">
-        <v>0.913453055738505</v>
+        <v>0.9254161399106554</v>
       </c>
     </row>
     <row r="20">
@@ -1238,40 +1238,40 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.7401925472774288</v>
+        <v>0.7368214919896041</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9995836396024131</v>
+        <v>0.9995937724564025</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8471407025044886</v>
+        <v>0.8428689213657525</v>
       </c>
       <c r="E20" t="n">
-        <v>0.812052230317157</v>
+        <v>0.8125134423108428</v>
       </c>
       <c r="F20" t="n">
-        <v>0.7804145244215939</v>
+        <v>0.7949558161953727</v>
       </c>
       <c r="G20" t="n">
-        <v>0.9192975669283413</v>
+        <v>0.9250841546612606</v>
       </c>
       <c r="H20" t="n">
-        <v>0.8957718251115565</v>
+        <v>0.902677396697679</v>
       </c>
       <c r="I20" t="n">
-        <v>0.8289976756275277</v>
+        <v>0.8041209327085042</v>
       </c>
       <c r="J20" t="n">
-        <v>0.911268257353237</v>
+        <v>0.9113880357241321</v>
       </c>
       <c r="K20" t="n">
-        <v>0.891255697073622</v>
+        <v>0.8884343059723382</v>
       </c>
       <c r="L20" t="n">
-        <v>0.9132050199992661</v>
+        <v>0.8820559337272027</v>
       </c>
       <c r="M20" t="n">
-        <v>0.9146147403952604</v>
+        <v>0.9216573538120314</v>
       </c>
     </row>
     <row r="21">
@@ -1279,40 +1279,40 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.7277182468870356</v>
+        <v>0.7334247097230463</v>
       </c>
       <c r="C21" t="n">
-        <v>0.9996412398822739</v>
+        <v>0.9995777596927741</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8545045798971426</v>
+        <v>0.8469409976872281</v>
       </c>
       <c r="E21" t="n">
-        <v>0.7890397706052669</v>
+        <v>0.8061279079066799</v>
       </c>
       <c r="F21" t="n">
-        <v>0.792340938303342</v>
+        <v>0.7292424485861182</v>
       </c>
       <c r="G21" t="n">
-        <v>0.9197428273090638</v>
+        <v>0.9250412461180124</v>
       </c>
       <c r="H21" t="n">
-        <v>0.904342326619028</v>
+        <v>0.90579745712686</v>
       </c>
       <c r="I21" t="n">
-        <v>0.7935382637446899</v>
+        <v>0.8140425151651132</v>
       </c>
       <c r="J21" t="n">
-        <v>0.9102003111629716</v>
+        <v>0.9148016261543803</v>
       </c>
       <c r="K21" t="n">
-        <v>0.8939276105006657</v>
+        <v>0.8970500722005369</v>
       </c>
       <c r="L21" t="n">
-        <v>0.9860830795200176</v>
+        <v>0.8840891159957432</v>
       </c>
       <c r="M21" t="n">
-        <v>0.9195473486312435</v>
+        <v>0.9177059650606652</v>
       </c>
     </row>
   </sheetData>

</xml_diff>